<commit_message>
update fertilizer 2020 ok
</commit_message>
<xml_diff>
--- a/data-raw/rural-yearbook/part03-agri-produce/02-fertilizer/raw-2018-2019-unlocked.xlsx
+++ b/data-raw/rural-yearbook/part03-agri-produce/02-fertilizer/raw-2018-2019-unlocked.xlsx
@@ -1,32 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\techme\data-raw\rural-yearbook\part03-agri-produce\02-fertilizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4F2C1FC-EDA3-4036-B694-BB9B197EC0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C17CB40-27F3-4935-9830-D202DE06273C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="DC32" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-24120" yWindow="3090" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-2" sheetId="1" r:id="rId1"/>
     <sheet name="CNKI" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -690,9 +681,6 @@
     <t>3-11 续表</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>3.钾肥</t>
   </si>
   <si>
@@ -1009,13 +997,17 @@
   </si>
   <si>
     <t>http://www.cnki.net/</t>
+  </si>
+  <si>
+    <t>地区</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1042,6 +1034,12 @@
       <sz val="12"/>
       <color indexed="12"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -1212,7 +1210,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1280,6 +1278,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1596,10 +1597,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1659,15 +1662,15 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>219</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>220</v>
       </c>
       <c r="L3" s="21"/>
       <c r="M3" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N3" s="22"/>
     </row>
@@ -1725,16 +1728,16 @@
         <v>9</v>
       </c>
       <c r="K5" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="L5" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -1772,7 +1775,7 @@
         <v>203</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -1801,13 +1804,13 @@
         <v>23</v>
       </c>
       <c r="K7" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>228</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>229</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>91</v>
@@ -1839,16 +1842,16 @@
         <v>30</v>
       </c>
       <c r="K8" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="L8" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>232</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -1877,16 +1880,16 @@
         <v>37</v>
       </c>
       <c r="K9" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="L9" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="M9" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="N9" s="13" t="s">
         <v>236</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -1915,16 +1918,16 @@
         <v>44</v>
       </c>
       <c r="K10" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="L10" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="M10" s="13" t="s">
+      <c r="N10" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
@@ -1950,19 +1953,19 @@
         <v>50</v>
       </c>
       <c r="J11" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="M11" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="M11" s="13" t="s">
+      <c r="N11" s="13" t="s">
         <v>244</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -1991,16 +1994,16 @@
         <v>58</v>
       </c>
       <c r="K12" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="L12" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="M12" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="M12" s="13" t="s">
+      <c r="N12" s="13" t="s">
         <v>248</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -2029,16 +2032,16 @@
         <v>65</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L13" s="13" t="s">
         <v>109</v>
       </c>
       <c r="M13" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="N13" s="13" t="s">
         <v>251</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
@@ -2076,7 +2079,7 @@
         <v>75</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -2105,16 +2108,16 @@
         <v>78</v>
       </c>
       <c r="K15" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="L15" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="M15" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="N15" s="13" t="s">
         <v>256</v>
-      </c>
-      <c r="N15" s="13" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.15">
@@ -2143,13 +2146,13 @@
         <v>85</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>64</v>
       </c>
       <c r="M16" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N16" s="13" t="s">
         <v>36</v>
@@ -2181,16 +2184,16 @@
         <v>92</v>
       </c>
       <c r="K17" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="L17" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="M17" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="M17" s="13" t="s">
+      <c r="N17" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="N17" s="13" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
@@ -2219,16 +2222,16 @@
         <v>99</v>
       </c>
       <c r="K18" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="L18" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="M18" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="N18" s="13" t="s">
         <v>266</v>
-      </c>
-      <c r="N18" s="13" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.15">
@@ -2263,10 +2266,10 @@
         <v>25</v>
       </c>
       <c r="M19" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="N19" s="13" t="s">
         <v>268</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
@@ -2295,16 +2298,16 @@
         <v>112</v>
       </c>
       <c r="K20" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="M20" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="N20" s="13" t="s">
         <v>272</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.15">
@@ -2333,16 +2336,16 @@
         <v>119</v>
       </c>
       <c r="K21" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="L21" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="M21" s="13" t="s">
+      <c r="N21" s="13" t="s">
         <v>276</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.15">
@@ -2371,16 +2374,16 @@
         <v>126</v>
       </c>
       <c r="K22" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="L22" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="L22" s="13" t="s">
+      <c r="M22" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="M22" s="13" t="s">
+      <c r="N22" s="13" t="s">
         <v>280</v>
-      </c>
-      <c r="N22" s="13" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
@@ -2409,16 +2412,16 @@
         <v>133</v>
       </c>
       <c r="K23" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="L23" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="L23" s="13" t="s">
+      <c r="M23" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="M23" s="13" t="s">
+      <c r="N23" s="13" t="s">
         <v>284</v>
-      </c>
-      <c r="N23" s="13" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
@@ -2447,16 +2450,16 @@
         <v>140</v>
       </c>
       <c r="K24" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="M24" s="13" t="s">
+      <c r="N24" s="13" t="s">
         <v>288</v>
-      </c>
-      <c r="N24" s="13" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.15">
@@ -2485,16 +2488,16 @@
         <v>147</v>
       </c>
       <c r="K25" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="L25" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="M25" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="M25" s="13" t="s">
+      <c r="N25" s="13" t="s">
         <v>292</v>
-      </c>
-      <c r="N25" s="13" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.15">
@@ -2526,13 +2529,13 @@
         <v>90</v>
       </c>
       <c r="L26" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="M26" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="M26" s="13" t="s">
+      <c r="N26" s="13" t="s">
         <v>295</v>
-      </c>
-      <c r="N26" s="13" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.15">
@@ -2567,10 +2570,10 @@
         <v>27</v>
       </c>
       <c r="M27" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="N27" s="13" t="s">
         <v>297</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.15">
@@ -2602,13 +2605,13 @@
         <v>195</v>
       </c>
       <c r="L28" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="M28" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="N28" s="13" t="s">
         <v>300</v>
-      </c>
-      <c r="N28" s="13" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
@@ -2637,16 +2640,16 @@
         <v>171</v>
       </c>
       <c r="K29" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="L29" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="M29" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="M29" s="13" t="s">
+      <c r="N29" s="13" t="s">
         <v>304</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
@@ -2675,16 +2678,16 @@
         <v>177</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L30" s="13" t="s">
         <v>36</v>
       </c>
       <c r="M30" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="N30" s="13" t="s">
         <v>307</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
@@ -2719,10 +2722,10 @@
         <v>21</v>
       </c>
       <c r="M31" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="N31" s="13" t="s">
         <v>309</v>
-      </c>
-      <c r="N31" s="13" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
@@ -2751,16 +2754,16 @@
         <v>189</v>
       </c>
       <c r="K32" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="L32" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="M32" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="M32" s="13" t="s">
+      <c r="N32" s="13" t="s">
         <v>313</v>
-      </c>
-      <c r="N32" s="13" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.15">
@@ -2786,16 +2789,16 @@
         <v>195</v>
       </c>
       <c r="J33" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="K33" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="K33" s="12" t="s">
-        <v>316</v>
-      </c>
       <c r="L33" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N33" s="13" t="s">
         <v>146</v>
@@ -2827,16 +2830,16 @@
         <v>201</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
@@ -2865,13 +2868,13 @@
         <v>207</v>
       </c>
       <c r="K35" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>318</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="M35" s="13" t="s">
         <v>319</v>
-      </c>
-      <c r="M35" s="13" t="s">
-        <v>320</v>
       </c>
       <c r="N35" s="13" t="s">
         <v>104</v>
@@ -2903,16 +2906,16 @@
         <v>212</v>
       </c>
       <c r="K36" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="L36" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="L36" s="16" t="s">
+      <c r="M36" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="M36" s="16" t="s">
+      <c r="N36" s="16" t="s">
         <v>323</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
@@ -2956,7 +2959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2965,13 +2968,13 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>